<commit_message>
Changed board outline and mounting to better fit inside enclosure
</commit_message>
<xml_diff>
--- a/product V2/Assembly/BOM.xlsx
+++ b/product V2/Assembly/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-zamorr.REDMOND\ESPDNS-Hardware\product V2\Assembly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach\Documents\Kicad\EsperDNS\ESPDNS-Hardware\product V2\Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5964EF10-75DE-4E0C-BB76-DEBDB075FB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BA0987-0845-40E2-9CDF-565E9E803A85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3349FBFB-726B-40FF-9ADF-BE26D3BA199E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3349FBFB-726B-40FF-9ADF-BE26D3BA199E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Item</t>
   </si>
@@ -51,12 +50,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>LCSC Part Number</t>
-  </si>
-  <si>
-    <t>C1, C13</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -75,12 +68,6 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>C4, C6</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -186,66 +173,18 @@
     <t>Package_DFN_QFN:QFN-24-1EP_4x4mm_P0.5mm_EP2.6x2.6mm</t>
   </si>
   <si>
-    <t>C45223</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
     <t>ESP32-WROOM-32D</t>
   </si>
   <si>
-    <t>Do Not Place</t>
-  </si>
-  <si>
-    <t>C19702</t>
-  </si>
-  <si>
-    <t>C15849</t>
-  </si>
-  <si>
-    <t>C14663</t>
-  </si>
-  <si>
-    <t>C19666</t>
-  </si>
-  <si>
-    <t>C72043</t>
-  </si>
-  <si>
-    <t>C21189</t>
-  </si>
-  <si>
-    <t>C23179</t>
-  </si>
-  <si>
-    <t>C25804</t>
-  </si>
-  <si>
-    <t>C23185</t>
-  </si>
-  <si>
-    <t>C22966</t>
-  </si>
-  <si>
-    <t>C8545</t>
-  </si>
-  <si>
-    <t>C22775</t>
-  </si>
-  <si>
     <t>R24</t>
   </si>
   <si>
     <t>R22, R23</t>
   </si>
   <si>
-    <t>C23255</t>
-  </si>
-  <si>
-    <t>C23182</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -253,6 +192,36 @@
   </si>
   <si>
     <t>TH</t>
+  </si>
+  <si>
+    <t>C1, C4, C6, C13</t>
+  </si>
+  <si>
+    <t>My Footprints:CLP6C-FKB</t>
+  </si>
+  <si>
+    <t>Inductor_SMD:L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>MountingHole:MountingHole_2.2mm_M2_Pad</t>
+  </si>
+  <si>
+    <t>digikey-footprints:USB_Micro_B_Female_10118192</t>
+  </si>
+  <si>
+    <t>My Footprints:ARJM11A3-009-AB-ER2-T</t>
+  </si>
+  <si>
+    <t>Connector_PinSocket_2.54mm:PinSocket_2x05_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>1-1825027-1:1-1825027-1</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-223</t>
+  </si>
+  <si>
+    <t>RF_Module:ESP32-WROOM-32</t>
   </si>
 </sst>
 </file>
@@ -621,18 +590,21 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.77734375" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1"/>
-    <col min="5" max="5" width="53.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="63" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="31.5703125" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,36 +621,32 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -686,22 +654,20 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -709,45 +675,41 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -755,22 +717,20 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -778,62 +738,62 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -841,20 +801,20 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -862,64 +822,62 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -927,135 +885,125 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1">
-        <v>0</v>
+        <v>470</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1">
-        <v>470</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="1">
-        <v>100</v>
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="D18" s="1">
+        <v>49.9</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1">
-        <v>49.9</v>
+        <v>270</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1063,171 +1011,134 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D20" s="1">
-        <v>270</v>
+        <v>47</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="D21" s="1">
+        <v>82</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="1">
-        <v>82</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G25" r:id="rId1" display="https://lcsc.com/product-detail/Ethernet-ICs_LAN8720A-CP-TR_C45223.html/?href=jlc-SMT" xr:uid="{F91FB432-CAC8-4540-8071-158225D734D6}"/>
-    <hyperlink ref="G2" r:id="rId2" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL10A106KP8NNNC_10uF-106-10-10V_C19702.html/?href=jlc-SMT" xr:uid="{16D4AC17-0BF6-4C59-8AA7-556BA4BEF1B7}"/>
-    <hyperlink ref="G4" r:id="rId3" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL10A105KB8NNNC_1uF-105-10-50V_C15849.html/?href=jlc-SMT" xr:uid="{1A06AE1E-1268-4214-B081-7A2276F2D02A}"/>
-    <hyperlink ref="G3" r:id="rId4" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_100nF-104-10-50V_C14663.html/?href=jlc-SMT" xr:uid="{4A213587-EA15-41A4-98C2-C33E2EBD9576}"/>
-    <hyperlink ref="G5" r:id="rId5" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL10A475KO8NNNC_4-7uF-475-10-16V_C19666.html/?href=jlc-SMT" xr:uid="{4A4AB19A-475E-4319-A5C4-A89D7D1BBAD8}"/>
-    <hyperlink ref="G6" r:id="rId6" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Green-light_C72043.html/?href=jlc-SMT" xr:uid="{03F08EDA-6231-4235-9875-AACE36B1D1CE}"/>
-    <hyperlink ref="G14" r:id="rId7" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0603WAF0000T5E_C21189.html/?href=jlc-SMT" xr:uid="{0E274368-B64D-4D4E-BB17-C94F5A47C4EE}"/>
-    <hyperlink ref="G15" r:id="rId8" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0603WAF4700T5E_C23179.html/?href=jlc-SMT" xr:uid="{725FC926-4821-47CB-B9AB-0A5B4FB60E20}"/>
-    <hyperlink ref="G17" r:id="rId9" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0603WAF1002T5E_C25804.html/?href=jlc-SMT" xr:uid="{3B9900FD-A713-42AB-A820-725F9FCF72DB}"/>
-    <hyperlink ref="G19" r:id="rId10" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0603WAF499JT5E_C23185.html/?href=jlc-SMT" xr:uid="{A345767A-0D27-457E-B0D2-1CC3032027D1}"/>
-    <hyperlink ref="G20" r:id="rId11" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0603WAF2700T5E_C22966.html/?href=jlc-SMT" xr:uid="{D550F78E-A399-42D4-9230-7FC35ABC1061}"/>
-    <hyperlink ref="G13" r:id="rId12" display="https://lcsc.com/product-detail/MOSFET_Changjiang-Electronics-Tech-CJ-2N7002_C8545.html/?href=jlc-SMT" xr:uid="{4CAC7CE4-2738-49D5-8BBE-58E9CE1908AC}"/>
-    <hyperlink ref="G16" r:id="rId13" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0603WAF1000T5E_C22775.html/?href=jlc-SMT" xr:uid="{D20480FB-F144-4BC8-A1C8-4DB11007AAC5}"/>
-    <hyperlink ref="G22" r:id="rId14" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0603WAF820JT5E_C23255.html/?href=jlc-SMT" xr:uid="{CA3BD40D-32DF-42A8-88EA-4C6DA55B3F44}"/>
-    <hyperlink ref="G21" r:id="rId15" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0603WAF470JT5E_C23182.html/?href=jlc-SMT" xr:uid="{4887765A-28FF-407F-9950-534B88DDD83A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>